<commit_message>
deus no ceu caputo na terra
</commit_message>
<xml_diff>
--- a/testeBot.xlsx
+++ b/testeBot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>J.A COMÉRCIO</t>
+          <t>Loja Kings Mauá</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(11) 4543-1550</t>
+          <t>(11) 4541-5875</t>
         </is>
       </c>
     </row>
@@ -476,19 +476,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>JO-COMÉRCIO DE ABRASIVOS E FERRAMENTAS LTDA</t>
+          <t>JS Calçados &amp; Roupas</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Loja de ferramentas</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>(11) 4555-1002</t>
-        </is>
-      </c>
+          <t>Loja de calçado</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -496,53 +492,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Maua Comercio De Livros E Informatica Ltda.</t>
+          <t>Rosi calçados</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Livraria</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Erorrima Indústria Comércio e Manu Equipamentos Mecânicos</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Loja de materiais de construção</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>(11) 4541-7941</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Jacobloja - Comércio de Cosméticos</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Perfumaria</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>(11) 98234-0537</t>
+          <t>Loja de calçado</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(11) 94310-5100</t>
         </is>
       </c>
     </row>

</xml_diff>